<commit_message>
Added Mounted Tire Processing Pipeline
</commit_message>
<xml_diff>
--- a/Person_B_and_trucks/on_trucks/Processed_Standalone/14_245-70R19.xlsx
+++ b/Person_B_and_trucks/on_trucks/Processed_Standalone/14_245-70R19.xlsx
@@ -1948,103 +1948,103 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>0</v>
+        <v>0.009721307704564801</v>
       </c>
       <c r="AR6">
-        <v>0.223246777998668</v>
+        <v>0.2252274311889522</v>
       </c>
       <c r="AS6">
-        <v>0.1347025873881126</v>
+        <v>0.1358976734352286</v>
       </c>
       <c r="AT6">
-        <v>0.2181735629871719</v>
+        <v>0.2201092064371697</v>
       </c>
       <c r="AU6">
-        <v>0.01174227507609177</v>
+        <v>0.01184645294956054</v>
       </c>
       <c r="AV6">
-        <v>0.009195967321217115</v>
+        <v>0.00927755426359452</v>
       </c>
       <c r="AW6">
-        <v>0.0005034000952110847</v>
+        <v>0.000507866278389662</v>
       </c>
       <c r="AX6">
-        <v>0.1265407682587021</v>
+        <v>0.1276634423622187</v>
       </c>
       <c r="AY6">
-        <v>0.05617059619053</v>
+        <v>0.05666894367640326</v>
       </c>
       <c r="AZ6">
-        <v>0.05308185065959252</v>
+        <v>0.0535527946875316</v>
       </c>
       <c r="BA6">
-        <v>0.003202036977778243</v>
+        <v>0.003230445561374833</v>
       </c>
       <c r="BB6">
-        <v>0.003099623613695048</v>
+        <v>0.003127123582358345</v>
       </c>
       <c r="BC6">
-        <v>0.006534066280422819</v>
+        <v>0.00659203674404996</v>
       </c>
       <c r="BD6">
-        <v>0.001063958216731477</v>
+        <v>0.001073397691088912</v>
       </c>
       <c r="BE6">
-        <v>0.004403899190271915</v>
+        <v>0.004442970737279658</v>
       </c>
       <c r="BF6">
-        <v>0.005908773701796164</v>
+        <v>0.005961196547886244</v>
       </c>
       <c r="BG6">
-        <v>0.0004375472663692388</v>
+        <v>0.0004414292009566197</v>
       </c>
       <c r="BH6">
-        <v>0.01578577610639678</v>
+        <v>0.01592582806184508</v>
       </c>
       <c r="BI6">
-        <v>0.006704223781297329</v>
+        <v>0.006763703888198962</v>
       </c>
       <c r="BJ6">
-        <v>0.0003381909325252729</v>
+        <v>0.0003411913742581223</v>
       </c>
       <c r="BK6">
-        <v>0.02883040901600405</v>
+        <v>0.02908619340898234</v>
       </c>
       <c r="BL6">
-        <v>0.03240346678072314</v>
+        <v>0.03269095146664273</v>
       </c>
       <c r="BM6">
-        <v>0.002475035819328574</v>
+        <v>0.002496994423325315</v>
       </c>
       <c r="BN6">
-        <v>0.01421128806915033</v>
+        <v>0.01433737111189139</v>
       </c>
       <c r="BO6">
-        <v>0.0008569314440542653</v>
+        <v>0.0008645341696735846</v>
       </c>
       <c r="BP6">
-        <v>0.005954239813400096</v>
+        <v>0.006007066036415949</v>
       </c>
       <c r="BQ6">
-        <v>0.003446600309258671</v>
+        <v>0.00347717866725051</v>
       </c>
       <c r="BR6">
-        <v>0.0005414345190897467</v>
+        <v>0.0005462381450017476</v>
       </c>
       <c r="BS6">
-        <v>0.006211289686732841</v>
+        <v>0.006266396465178174</v>
       </c>
       <c r="BT6">
-        <v>0.003088568536573119</v>
+        <v>0.003115970424207133</v>
       </c>
       <c r="BU6">
-        <v>0.002111207253124406</v>
+        <v>0.002129937957409316</v>
       </c>
       <c r="BV6">
-        <v>0.0006038142897018868</v>
+        <v>0.0006091713511115005</v>
       </c>
       <c r="BW6">
-        <v>0.0184298324202772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:75">
@@ -3083,103 +3083,103 @@
         <v>0</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>0.003326798909701525</v>
       </c>
       <c r="AR11">
-        <v>0.2945010927386066</v>
+        <v>0.3027048058516318</v>
       </c>
       <c r="AS11">
-        <v>0.09771066053687859</v>
+        <v>0.1004325187808486</v>
       </c>
       <c r="AT11">
-        <v>0.2057252104147719</v>
+        <v>0.2114559552166512</v>
       </c>
       <c r="AU11">
-        <v>0.01557321129169069</v>
+        <v>0.01600702346025521</v>
       </c>
       <c r="AV11">
-        <v>0.00352068767261901</v>
+        <v>0.00361876103240911</v>
       </c>
       <c r="AW11">
-        <v>0.002273184648482908</v>
+        <v>0.002336507179939995</v>
       </c>
       <c r="AX11">
-        <v>0.07843114332949198</v>
+        <v>0.08061594540617836</v>
       </c>
       <c r="AY11">
-        <v>0.02072393410740649</v>
+        <v>0.02130122639657739</v>
       </c>
       <c r="AZ11">
-        <v>0.05774299577384605</v>
+        <v>0.05935150244256566</v>
       </c>
       <c r="BA11">
-        <v>0.0108507835304889</v>
+        <v>0.011153046297353</v>
       </c>
       <c r="BB11">
-        <v>2.708553366157931E-05</v>
+        <v>2.784003662659889E-05</v>
       </c>
       <c r="BC11">
-        <v>0.01677939586542765</v>
+        <v>0.01724680788284936</v>
       </c>
       <c r="BD11">
-        <v>0.01257204397400565</v>
+        <v>0.0129222547017418</v>
       </c>
       <c r="BE11">
-        <v>0.03515048593735561</v>
+        <v>0.03612964869608071</v>
       </c>
       <c r="BF11">
-        <v>0.008932756234424303</v>
+        <v>0.009181589842389377</v>
       </c>
       <c r="BG11">
-        <v>0.0007025625441254645</v>
+        <v>0.0007221333426660258</v>
       </c>
       <c r="BH11">
-        <v>0.01718763237011445</v>
+        <v>0.01766641634930232</v>
       </c>
       <c r="BI11">
-        <v>0.002896729489078782</v>
+        <v>0.002977421677598215</v>
       </c>
       <c r="BJ11">
-        <v>0.002594886153465553</v>
+        <v>0.002667170101093848</v>
       </c>
       <c r="BK11">
-        <v>0.0424554230967461</v>
+        <v>0.04363807443409427</v>
       </c>
       <c r="BL11">
-        <v>0.02249858965191356</v>
+        <v>0.02312531729232948</v>
       </c>
       <c r="BM11">
-        <v>0.0001056410992753355</v>
+        <v>0.0001085838702625002</v>
       </c>
       <c r="BN11">
-        <v>0.002250205809783782</v>
+        <v>0.002312888235635131</v>
       </c>
       <c r="BO11">
-        <v>0.0003939916443419537</v>
+        <v>0.0004049667968925057</v>
       </c>
       <c r="BP11">
-        <v>0.0008161860692180302</v>
+        <v>0.0008389219996570237</v>
       </c>
       <c r="BQ11">
-        <v>0.002242357746053525</v>
+        <v>0.00230482155382527</v>
       </c>
       <c r="BR11">
-        <v>0.0002339532016064927</v>
+        <v>0.0002404702740221015</v>
       </c>
       <c r="BS11">
-        <v>0.005944883694113478</v>
+        <v>0.006110486204662043</v>
       </c>
       <c r="BT11">
-        <v>0.001166639490389394</v>
+        <v>0.001199137759229352</v>
       </c>
       <c r="BU11">
-        <v>0.003642396199683159</v>
+        <v>0.003743859909675896</v>
       </c>
       <c r="BV11">
-        <v>0.004015248078527668</v>
+        <v>0.004127098065254554</v>
       </c>
       <c r="BW11">
-        <v>0.0303380020724051</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4458,103 +4458,103 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>0</v>
+        <v>0.009721307704564801</v>
       </c>
       <c r="AR6">
-        <v>0.223246777998668</v>
+        <v>0.2349487388935171</v>
       </c>
       <c r="AS6">
-        <v>0.3579493653867806</v>
+        <v>0.3708464123287457</v>
       </c>
       <c r="AT6">
-        <v>0.5761229283739526</v>
+        <v>0.5909556187659153</v>
       </c>
       <c r="AU6">
-        <v>0.5878652034500444</v>
+        <v>0.6028020717154758</v>
       </c>
       <c r="AV6">
-        <v>0.5970611707712615</v>
+        <v>0.6120796259790704</v>
       </c>
       <c r="AW6">
-        <v>0.5975645708664726</v>
+        <v>0.61258749225746</v>
       </c>
       <c r="AX6">
-        <v>0.7241053391251748</v>
+        <v>0.7402509346196787</v>
       </c>
       <c r="AY6">
-        <v>0.7802759353157048</v>
+        <v>0.796919878296082</v>
       </c>
       <c r="AZ6">
-        <v>0.8333577859752973</v>
+        <v>0.8504726729836136</v>
       </c>
       <c r="BA6">
-        <v>0.8365598229530755</v>
+        <v>0.8537031185449885</v>
       </c>
       <c r="BB6">
-        <v>0.8396594465667706</v>
+        <v>0.8568302421273468</v>
       </c>
       <c r="BC6">
-        <v>0.8461935128471935</v>
+        <v>0.8634222788713968</v>
       </c>
       <c r="BD6">
-        <v>0.8472574710639249</v>
+        <v>0.8644956765624857</v>
       </c>
       <c r="BE6">
-        <v>0.8516613702541969</v>
+        <v>0.8689386472997653</v>
       </c>
       <c r="BF6">
-        <v>0.8575701439559931</v>
+        <v>0.8748998438476516</v>
       </c>
       <c r="BG6">
-        <v>0.8580076912223623</v>
+        <v>0.8753412730486082</v>
       </c>
       <c r="BH6">
-        <v>0.8737934673287591</v>
+        <v>0.8912671011104533</v>
       </c>
       <c r="BI6">
-        <v>0.8804976911100564</v>
+        <v>0.8980308049986522</v>
       </c>
       <c r="BJ6">
-        <v>0.8808358820425817</v>
+        <v>0.8983719963729103</v>
       </c>
       <c r="BK6">
-        <v>0.9096662910585858</v>
+        <v>0.9274581897818927</v>
       </c>
       <c r="BL6">
-        <v>0.9420697578393089</v>
+        <v>0.9601491412485353</v>
       </c>
       <c r="BM6">
-        <v>0.9445447936586375</v>
+        <v>0.9626461356718606</v>
       </c>
       <c r="BN6">
-        <v>0.9587560817277878</v>
+        <v>0.976983506783752</v>
       </c>
       <c r="BO6">
-        <v>0.9596130131718421</v>
+        <v>0.9778480409534256</v>
       </c>
       <c r="BP6">
-        <v>0.9655672529852422</v>
+        <v>0.9838551069898416</v>
       </c>
       <c r="BQ6">
-        <v>0.9690138532945008</v>
+        <v>0.9873322856570921</v>
       </c>
       <c r="BR6">
-        <v>0.9695552878135906</v>
+        <v>0.9878785238020938</v>
       </c>
       <c r="BS6">
-        <v>0.9757665775003234</v>
+        <v>0.994144920267272</v>
       </c>
       <c r="BT6">
-        <v>0.9788551460368965</v>
+        <v>0.9972608906914791</v>
       </c>
       <c r="BU6">
-        <v>0.9809663532900209</v>
+        <v>0.9993908286488884</v>
       </c>
       <c r="BV6">
-        <v>0.9815701675797228</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="BW6">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:75">
@@ -5593,103 +5593,103 @@
         <v>0</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>0.003326798909701525</v>
       </c>
       <c r="AR11">
-        <v>0.2945010927386066</v>
+        <v>0.3060316047613333</v>
       </c>
       <c r="AS11">
-        <v>0.3922117532754852</v>
+        <v>0.4064641235421819</v>
       </c>
       <c r="AT11">
-        <v>0.5979369636902571</v>
+        <v>0.6179200787588331</v>
       </c>
       <c r="AU11">
-        <v>0.6135101749819477</v>
+        <v>0.6339271022190883</v>
       </c>
       <c r="AV11">
-        <v>0.6170308626545667</v>
+        <v>0.6375458632514974</v>
       </c>
       <c r="AW11">
-        <v>0.6193040473030497</v>
+        <v>0.6398823704314374</v>
       </c>
       <c r="AX11">
-        <v>0.6977351906325416</v>
+        <v>0.7204983158376157</v>
       </c>
       <c r="AY11">
-        <v>0.7184591247399481</v>
+        <v>0.7417995422341931</v>
       </c>
       <c r="AZ11">
-        <v>0.7762021205137941</v>
+        <v>0.8011510446767588</v>
       </c>
       <c r="BA11">
-        <v>0.787052904044283</v>
+        <v>0.8123040909741118</v>
       </c>
       <c r="BB11">
-        <v>0.7870799895779446</v>
+        <v>0.8123319310107384</v>
       </c>
       <c r="BC11">
-        <v>0.8038593854433722</v>
+        <v>0.8295787388935878</v>
       </c>
       <c r="BD11">
-        <v>0.8164314294173779</v>
+        <v>0.8425009935953296</v>
       </c>
       <c r="BE11">
-        <v>0.8515819153547335</v>
+        <v>0.8786306422914103</v>
       </c>
       <c r="BF11">
-        <v>0.8605146715891578</v>
+        <v>0.8878122321337997</v>
       </c>
       <c r="BG11">
-        <v>0.8612172341332833</v>
+        <v>0.8885343654764657</v>
       </c>
       <c r="BH11">
-        <v>0.8784048665033978</v>
+        <v>0.906200781825768</v>
       </c>
       <c r="BI11">
-        <v>0.8813015959924766</v>
+        <v>0.9091782035033662</v>
       </c>
       <c r="BJ11">
-        <v>0.8838964821459422</v>
+        <v>0.9118453736044601</v>
       </c>
       <c r="BK11">
-        <v>0.9263519052426883</v>
+        <v>0.9554834480385543</v>
       </c>
       <c r="BL11">
-        <v>0.9488504948946018</v>
+        <v>0.9786087653308838</v>
       </c>
       <c r="BM11">
-        <v>0.9489561359938772</v>
+        <v>0.9787173492011463</v>
       </c>
       <c r="BN11">
-        <v>0.9512063418036609</v>
+        <v>0.9810302374367814</v>
       </c>
       <c r="BO11">
-        <v>0.9516003334480029</v>
+        <v>0.9814352042336739</v>
       </c>
       <c r="BP11">
-        <v>0.9524165195172209</v>
+        <v>0.982274126233331</v>
       </c>
       <c r="BQ11">
-        <v>0.9546588772632745</v>
+        <v>0.9845789477871563</v>
       </c>
       <c r="BR11">
-        <v>0.9548928304648809</v>
+        <v>0.9848194180611783</v>
       </c>
       <c r="BS11">
-        <v>0.9608377141589944</v>
+        <v>0.9909299042658404</v>
       </c>
       <c r="BT11">
-        <v>0.9620043536493839</v>
+        <v>0.9921290420250697</v>
       </c>
       <c r="BU11">
-        <v>0.9656467498490671</v>
+        <v>0.9958729019347455</v>
       </c>
       <c r="BV11">
-        <v>0.9696619979275948</v>
+        <v>1</v>
       </c>
       <c r="BW11">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.5761229283739526</v>
+        <v>0.5909556187659153</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -6132,7 +6132,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.5979369636902571</v>
+        <v>0.6179200787588331</v>
       </c>
       <c r="G11">
         <v>4</v>
@@ -6391,7 +6391,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.7241053391251748</v>
+        <v>0.7402509346196787</v>
       </c>
       <c r="G6">
         <v>8</v>
@@ -6590,16 +6590,16 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.7184591247399481</v>
+        <v>0.7204983158376157</v>
       </c>
       <c r="G11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <v>14</v>
@@ -6855,7 +6855,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.8333577859752973</v>
+        <v>0.8504726729836136</v>
       </c>
       <c r="G6">
         <v>10</v>
@@ -7054,16 +7054,16 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.8038593854433722</v>
+        <v>0.8011510446767588</v>
       </c>
       <c r="G11">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>14</v>
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.9096662910585858</v>
+        <v>0.9274581897818927</v>
       </c>
       <c r="G6">
         <v>21</v>
@@ -7518,16 +7518,16 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0.9263519052426883</v>
+        <v>0.906200781825768</v>
       </c>
       <c r="G11">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H11">
         <v>14</v>

</xml_diff>